<commit_message>
Field added in Notes API and same uploaded on production
</commit_message>
<xml_diff>
--- a/src/report/Layouts/VendorLedgerEntries.xlsx
+++ b/src/report/Layouts/VendorLedgerEntries.xlsx
@@ -1,54 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <x:workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://moonlightlb-my.sharepoint.com/personal/faisal_moonlight_com_lb/Documents/Documents/AL development/MASQ-Team/src/report/Layouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{C047C7D7-11EE-4DA8-AAC2-1AF211845798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD3B5AD1-9C15-41A4-8468-5E67CCB50858}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="TranslationData" sheetId="2" state="hidden" r:id="rId1"/>
-    <sheet name="CaptionData" sheetId="3" state="hidden" r:id="rId2"/>
-    <sheet name="Aggregated Metadata" sheetId="4" state="hidden" r:id="rId3"/>
-    <sheet name="VendorLedgerEntry" sheetId="5" r:id="rId4"/>
-  </sheets>
-  <definedNames>
-    <definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.CompanyDisplayName" comment="Use this function to get the Company display name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company display name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.LayoutCaption" comment="Use this function to get the Layout caption from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout caption",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.LayoutId" comment="Use this function to get the Layout id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.LayoutName" comment="Use this function to get the Layout name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-  </definedNames>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+  <x:bookViews>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="TranslationData" sheetId="2" state="hidden" r:id="rId1"/>
+    <x:sheet name="CaptionData" sheetId="3" state="hidden" r:id="rId2"/>
+    <x:sheet name="Aggregated Metadata" sheetId="4" state="hidden" r:id="rId3"/>
+    <x:sheet name="VendorLedgerEntry" sheetId="5" r:id="rId4"/>
+  </x:sheets>
+  <x:definedNames>
+    <x:definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.CompanyDisplayName" comment="Use this function to get the Company display name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company display name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.LayoutCaption" comment="Use this function to get the Layout caption from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout caption",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.LayoutId" comment="Use this function to get the Layout id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.LayoutName" comment="Use this function to get the Layout name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+  </x:definedNames>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -58,168 +55,168 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="151">
   <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
     <t>CaptionKey</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Caption</t>
   </si>
   <si>
+    <t>Request Page Option</t>
+  </si>
+  <si>
+    <t>Request Page Option Value</t>
+  </si>
+  <si>
+    <t>Report Property</t>
+  </si>
+  <si>
+    <t>Report Property Value</t>
+  </si>
+  <si>
+    <t>Extension ID</t>
+  </si>
+  <si>
+    <t>Extension ID Value</t>
+  </si>
+  <si>
+    <t>Extension Name</t>
+  </si>
+  <si>
+    <t>Extension Name Value</t>
+  </si>
+  <si>
+    <t>Extension Publisher</t>
+  </si>
+  <si>
+    <t>Extension Publisher Value</t>
+  </si>
+  <si>
+    <t>Extension Version</t>
+  </si>
+  <si>
+    <t>Extension Version Value</t>
+  </si>
+  <si>
+    <t>Object ID</t>
+  </si>
+  <si>
+    <t>Object ID Value</t>
+  </si>
+  <si>
+    <t>Object Name</t>
+  </si>
+  <si>
+    <t>Object Name Value</t>
+  </si>
+  <si>
+    <t>About This Report Title</t>
+  </si>
+  <si>
+    <t>About This Report Title Value</t>
+  </si>
+  <si>
+    <t>About This Report Text</t>
+  </si>
+  <si>
+    <t>About This Report Text Value</t>
+  </si>
+  <si>
+    <t>Report help link</t>
+  </si>
+  <si>
+    <t>Report help link Value</t>
+  </si>
+  <si>
+    <t>Request Property</t>
+  </si>
+  <si>
+    <t>Request Property Value</t>
+  </si>
+  <si>
+    <t>Tenant Id</t>
+  </si>
+  <si>
+    <t>Tenant Id Value</t>
+  </si>
+  <si>
+    <t>Environment name</t>
+  </si>
+  <si>
+    <t>Environment name Value</t>
+  </si>
+  <si>
+    <t>Environment type</t>
+  </si>
+  <si>
+    <t>Environment type Value</t>
+  </si>
+  <si>
+    <t>Company name</t>
+  </si>
+  <si>
+    <t>Company name Value</t>
+  </si>
+  <si>
+    <t>Company Id</t>
+  </si>
+  <si>
+    <t>Company Id Value</t>
+  </si>
+  <si>
+    <t>User name</t>
+  </si>
+  <si>
+    <t>User name Value</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Date Value</t>
+  </si>
+  <si>
+    <t>Language Value</t>
+  </si>
+  <si>
+    <t>Format Region</t>
+  </si>
+  <si>
+    <t>Format Region Value</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Filter Value</t>
+  </si>
+  <si>
     <t>CaptionValue</t>
   </si>
   <si>
-    <t>Report Property</t>
-  </si>
-  <si>
-    <t>Report Property Value</t>
-  </si>
-  <si>
-    <t>Request Property</t>
-  </si>
-  <si>
-    <t>Request Property Value</t>
-  </si>
-  <si>
-    <t>Request Page Option</t>
-  </si>
-  <si>
-    <t>Request Page Option Value</t>
-  </si>
-  <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>Filter Value</t>
-  </si>
-  <si>
-    <t>Extension ID</t>
-  </si>
-  <si>
-    <t>Extension ID Value</t>
-  </si>
-  <si>
     <t>Tenant Entra Id</t>
   </si>
   <si>
     <t>Tenant Entra Id Value</t>
   </si>
   <si>
-    <t>Extension Name</t>
-  </si>
-  <si>
-    <t>Extension Name Value</t>
-  </si>
-  <si>
-    <t>Tenant Id</t>
-  </si>
-  <si>
-    <t>Tenant Id Value</t>
-  </si>
-  <si>
-    <t>Extension Publisher</t>
-  </si>
-  <si>
-    <t>Extension Publisher Value</t>
-  </si>
-  <si>
-    <t>Environment name</t>
-  </si>
-  <si>
-    <t>Environment name Value</t>
-  </si>
-  <si>
-    <t>Extension Version</t>
-  </si>
-  <si>
-    <t>Extension Version Value</t>
-  </si>
-  <si>
-    <t>Environment type</t>
-  </si>
-  <si>
-    <t>Environment type Value</t>
-  </si>
-  <si>
-    <t>Object ID</t>
-  </si>
-  <si>
-    <t>Object ID Value</t>
-  </si>
-  <si>
-    <t>Company name</t>
-  </si>
-  <si>
-    <t>Company name Value</t>
-  </si>
-  <si>
-    <t>Object Name</t>
-  </si>
-  <si>
-    <t>Object Name Value</t>
-  </si>
-  <si>
     <t>Company display name</t>
   </si>
   <si>
     <t>Company display name Value</t>
-  </si>
-  <si>
-    <t>About This Report Title</t>
-  </si>
-  <si>
-    <t>About This Report Title Value</t>
-  </si>
-  <si>
-    <t>Company Id</t>
-  </si>
-  <si>
-    <t>Company Id Value</t>
-  </si>
-  <si>
-    <t>About This Report Text</t>
-  </si>
-  <si>
-    <t>About This Report Text Value</t>
-  </si>
-  <si>
-    <t>User name</t>
-  </si>
-  <si>
-    <t>User name Value</t>
-  </si>
-  <si>
-    <t>Report help link</t>
-  </si>
-  <si>
-    <t>Report help link Value</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Date Value</t>
-  </si>
-  <si>
-    <t>Language Value</t>
-  </si>
-  <si>
-    <t>Format Region</t>
-  </si>
-  <si>
-    <t>Format Region Value</t>
   </si>
   <si>
     <t>Layout name</t>
@@ -526,7 +523,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -717,6 +714,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DC11CF61-B374-4F0B-84B3-23694D65F56E}" name="TranslationData" displayName="TranslationData" ref="A1:C2" totalsRowShown="0">
   <autoFilter ref="A1:C2" xr:uid="{DC11CF61-B374-4F0B-84B3-23694D65F56E}"/>
@@ -785,108 +786,108 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="VendorLedgerEntry" displayName="VendorLedgerEntry" ref="A1:CL2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:CL2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="90">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AcceptedPaymentTolerance"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AcceptedPmtDiscTolerance"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AdjustedCurrencyFactor"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Amount"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmountLCY"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmounttoApply"/>
-    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AppliestoDocNo"/>
-    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AppliestoDocType"/>
-    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AppliestoExtDocNo"/>
-    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AppliestoID"/>
-    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ApplyingEntry"/>
-    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BalAccountNo"/>
-    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BalAccountType"/>
-    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BuyfromVendorNo"/>
-    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ClosedatDate"/>
-    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ClosedbyAmount"/>
-    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ClosedbyAmountLCY"/>
-    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ClosedbyCurrencyAmount"/>
-    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ClosedbyCurrencyCode"/>
-    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ClosedbyEntryNo"/>
-    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CreditAmount"/>
-    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CreditAmountLCY"/>
-    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CreditorNo"/>
-    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CurrencyCode"/>
-    <tableColumn id="25" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DebitAmount"/>
-    <tableColumn id="26" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DebitAmountLCY"/>
-    <tableColumn id="27" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Description"/>
-    <tableColumn id="28" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DimensionSetID"/>
-    <tableColumn id="29" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentDate"/>
-    <tableColumn id="30" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentNo"/>
-    <tableColumn id="31" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentType"/>
-    <tableColumn id="32" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DueDate"/>
-    <tableColumn id="33" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EmployeeDescription"/>
-    <tableColumn id="34" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EntryNo"/>
-    <tableColumn id="35" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ExportedtoPaymentFile"/>
-    <tableColumn id="36" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ExternalDocumentNo"/>
-    <tableColumn id="37" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="GlobalDimension1Code"/>
-    <tableColumn id="38" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="GlobalDimension2Code"/>
-    <tableColumn id="39" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ICPartnerCode"/>
-    <tableColumn id="40" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="InvDiscountLCY"/>
-    <tableColumn id="41" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="InvoiceReceivedDate"/>
-    <tableColumn id="42" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="JournalBatchName"/>
-    <tableColumn id="43" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="JournalTemplName"/>
-    <tableColumn id="44" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="MaxPaymentTolerance"/>
-    <tableColumn id="45" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="MessagetoRecipient"/>
-    <tableColumn id="46" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="NoSeries"/>
-    <tableColumn id="47" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OnHold"/>
-    <tableColumn id="48" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Open"/>
-    <tableColumn id="49" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OrigPmtDiscPossibleLCY"/>
-    <tableColumn id="50" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OriginalAmount"/>
-    <tableColumn id="51" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OriginalAmtLCY"/>
-    <tableColumn id="52" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OriginalCurrencyFactor"/>
-    <tableColumn id="53" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OriginalPmtDiscPossible"/>
-    <tableColumn id="54" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PaymentMethodCode"/>
-    <tableColumn id="55" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PaymentReference"/>
-    <tableColumn id="56" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PmtDiscRcdLCY"/>
-    <tableColumn id="57" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PmtDiscToleranceDate"/>
-    <tableColumn id="58" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PmtDiscountDate"/>
-    <tableColumn id="59" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PmtToleranceLCY"/>
-    <tableColumn id="60" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Positive"/>
-    <tableColumn id="61" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PostingDate"/>
-    <tableColumn id="62" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Prepayment"/>
-    <tableColumn id="63" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PurchaseLCY"/>
-    <tableColumn id="64" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PurchaserCode"/>
-    <tableColumn id="65" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReasonCode"/>
-    <tableColumn id="66" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RecipientBankAccount"/>
-    <tableColumn id="67" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RemainingAmount"/>
-    <tableColumn id="68" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RemainingAmtLCY"/>
-    <tableColumn id="69" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RemainingPmtDiscPossible"/>
-    <tableColumn id="70" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RemittoCode"/>
-    <tableColumn id="71" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Reversed"/>
-    <tableColumn id="72" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReversedEntryNo"/>
-    <tableColumn id="73" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReversedbyEntryNo"/>
-    <tableColumn id="74" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShortcutDimension3Code"/>
-    <tableColumn id="75" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShortcutDimension4Code"/>
-    <tableColumn id="76" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShortcutDimension5Code"/>
-    <tableColumn id="77" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShortcutDimension6Code"/>
-    <tableColumn id="78" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShortcutDimension7Code"/>
-    <tableColumn id="79" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShortcutDimension8Code"/>
-    <tableColumn id="80" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SourceCode"/>
-    <tableColumn id="81" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SystemCreatedAt"/>
-    <tableColumn id="82" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SystemCreatedBy"/>
-    <tableColumn id="83" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SystemId"/>
-    <tableColumn id="84" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SystemModifiedAt"/>
-    <tableColumn id="85" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SystemModifiedBy"/>
-    <tableColumn id="86" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="TransactionNo"/>
-    <tableColumn id="87" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UserID"/>
-    <tableColumn id="88" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="VendorName"/>
-    <tableColumn id="89" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="VendorNo"/>
-    <tableColumn id="90" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="VendorPostingGroup"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="VendorLedgerEntry" displayName="VendorLedgerEntry" ref="A1:CL2" totalsRowShown="0" headerRowDxfId="0" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+  <x:autoFilter ref="A1:CL2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <x:tableColumns count="90">
+    <x:tableColumn id="1" name="AcceptedPaymentTolerance" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="2" name="AcceptedPmtDiscTolerance" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="3" name="AdjustedCurrencyFactor" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="4" name="Amount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="5" name="AmountLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="6" name="AmounttoApply" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="7" name="AppliestoDocNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="8" name="AppliestoDocType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="9" name="AppliestoExtDocNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="10" name="AppliestoID" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="11" name="ApplyingEntry" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="12" name="BalAccountNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="13" name="BalAccountType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="14" name="BuyfromVendorNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="15" name="ClosedatDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="16" name="ClosedbyAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="17" name="ClosedbyAmountLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="18" name="ClosedbyCurrencyAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="19" name="ClosedbyCurrencyCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="20" name="ClosedbyEntryNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="21" name="CreditAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="22" name="CreditAmountLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="23" name="CreditorNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="24" name="CurrencyCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="25" name="DebitAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="26" name="DebitAmountLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="27" name="Description" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="28" name="DimensionSetID" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="29" name="DocumentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="30" name="DocumentNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="31" name="DocumentType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="32" name="DueDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="33" name="EmployeeDescription" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="34" name="EntryNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="35" name="ExportedtoPaymentFile" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="36" name="ExternalDocumentNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="37" name="GlobalDimension1Code" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="38" name="GlobalDimension2Code" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="39" name="ICPartnerCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="40" name="InvDiscountLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="41" name="InvoiceReceivedDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="42" name="JournalBatchName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="43" name="JournalTemplName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="44" name="MaxPaymentTolerance" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="45" name="MessagetoRecipient" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="46" name="NoSeries" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="47" name="OnHold" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="48" name="Open" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="49" name="OrigPmtDiscPossibleLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="50" name="OriginalAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="51" name="OriginalAmtLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="52" name="OriginalCurrencyFactor" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="53" name="OriginalPmtDiscPossible" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="54" name="PaymentMethodCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="55" name="PaymentReference" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="56" name="PmtDiscRcdLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="57" name="PmtDiscToleranceDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="58" name="PmtDiscountDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="59" name="PmtToleranceLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="60" name="Positive" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="61" name="PostingDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="62" name="Prepayment" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="63" name="PurchaseLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="64" name="PurchaserCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="65" name="ReasonCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="66" name="RecipientBankAccount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="67" name="RemainingAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="68" name="RemainingAmtLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="69" name="RemainingPmtDiscPossible" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="70" name="RemittoCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="71" name="Reversed" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="72" name="ReversedEntryNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="73" name="ReversedbyEntryNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="74" name="ShortcutDimension3Code" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="75" name="ShortcutDimension4Code" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="76" name="ShortcutDimension5Code" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="77" name="ShortcutDimension6Code" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="78" name="ShortcutDimension7Code" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="79" name="ShortcutDimension8Code" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="80" name="SourceCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="81" name="SystemCreatedAt" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="82" name="SystemCreatedBy" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="83" name="SystemId" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="84" name="SystemModifiedAt" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="85" name="SystemModifiedBy" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="86" name="TransactionNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="87" name="UserID" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="88" name="VendorName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="89" name="VendorNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="90" name="VendorPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -924,7 +925,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1030,7 +1031,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1172,7 +1173,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1186,21 +1187,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1219,26 +1220,26 @@
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1257,7 +1258,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
@@ -1272,187 +1273,187 @@
     <col min="11" max="11" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>52</v>
       </c>
@@ -1460,7 +1461,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>54</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>56</v>
       </c>
@@ -1493,12 +1494,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90">
+    <row r="1" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1770,7 +1771,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:90">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>

</xml_diff>